<commit_message>
Update week2 homework roster tab filter
</commit_message>
<xml_diff>
--- a/JasonL_Week2Homework.xlsx
+++ b/JasonL_Week2Homework.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teche\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teche\Code\SavvyCoders\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EE17B0-006B-422F-8471-B7A3ED6E264F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9341A-37AD-4766-9405-2ABC19C77313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -564,7 +564,7 @@
   <numFmts count="3">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -705,12 +705,12 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -745,7 +745,43 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="39">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -781,60 +817,6 @@
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1013,16 +995,70 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2024,49 +2060,55 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Payments!$A$5:$A$19</c:f>
+              <c:f>Payments!$A$5:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>1/2/2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1/5/2012</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1/15/2012</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1/16/2012</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>1/20/2012</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>1/21/2012</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1/26/2012</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1/31/2012</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2/2/2012</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>2/5/2012</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>2/15/2012</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>2/20/2012</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>2/25/2012</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>2/26/2012</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>2/27/2012</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>2/29/2012</c:v>
                 </c:pt>
               </c:strCache>
@@ -2074,47 +2116,53 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$B$5:$B$19</c:f>
+              <c:f>Payments!$B$5:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);\("$"#,##0.00\)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1392</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>6720</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>738.25</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>340</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>2200</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>6720</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>514</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>3770</c:v>
                 </c:pt>
               </c:numCache>
@@ -2152,49 +2200,55 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Payments!$A$5:$A$19</c:f>
+              <c:f>Payments!$A$5:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>1/2/2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1/5/2012</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1/15/2012</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1/16/2012</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>1/20/2012</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>1/21/2012</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1/26/2012</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1/31/2012</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2/2/2012</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>2/5/2012</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>2/15/2012</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>2/20/2012</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>2/25/2012</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>2/26/2012</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>2/27/2012</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>2/29/2012</c:v>
                 </c:pt>
               </c:strCache>
@@ -2202,26 +2256,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$C$5:$C$19</c:f>
+              <c:f>Payments!$C$5:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);\("$"#,##0.00\)</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
+                <c:ptCount val="16"/>
+                <c:pt idx="2">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>-20000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>-20000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>20000</c:v>
                 </c:pt>
               </c:numCache>
@@ -2259,49 +2313,55 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Payments!$A$5:$A$19</c:f>
+              <c:f>Payments!$A$5:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>1/2/2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1/5/2012</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1/15/2012</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1/16/2012</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>1/20/2012</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>1/21/2012</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1/26/2012</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1/31/2012</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2/2/2012</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>2/5/2012</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>2/15/2012</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>2/20/2012</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>2/25/2012</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>2/26/2012</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>2/27/2012</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>2/29/2012</c:v>
                 </c:pt>
               </c:strCache>
@@ -2309,23 +2369,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$D$5:$D$19</c:f>
+              <c:f>Payments!$D$5:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);\("$"#,##0.00\)</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="1">
+                <c:ptCount val="16"/>
+                <c:pt idx="3">
                   <c:v>105</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>-170</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>-70</c:v>
                 </c:pt>
               </c:numCache>
@@ -6785,8 +6845,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E87CAFBB-502F-4BEA-BFB3-36CE583846EA}" name="PivotTable7" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A3:E19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E87CAFBB-502F-4BEA-BFB3-36CE583846EA}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:E21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -6898,8 +6958,8 @@
         <item h="1" x="94"/>
         <item h="1" x="95"/>
         <item h="1" x="87"/>
-        <item h="1" x="90"/>
-        <item h="1" x="97"/>
+        <item x="90"/>
+        <item x="97"/>
         <item x="98"/>
         <item x="91"/>
         <item x="100"/>
@@ -6961,7 +7021,13 @@
   <rowFields count="1">
     <field x="8"/>
   </rowFields>
-  <rowItems count="15">
+  <rowItems count="17">
+    <i>
+      <x v="93"/>
+    </i>
+    <i>
+      <x v="94"/>
+    </i>
     <i>
       <x v="95"/>
     </i>
@@ -7029,48 +7095,48 @@
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="8" baseItem="0" numFmtId="7"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="11">
+    <format dxfId="23">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="22">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="21">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="20">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="17">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="16">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="15">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="14">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -7143,7 +7209,7 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{87B8A4D7-2B1E-436D-811B-E50528EF4688}" name="Credit Card"/>
     <tableColumn id="2" xr3:uid="{4AE103D0-BB6C-4FE9-9C2D-6C03FEB1A17F}" name="Balance"/>
-    <tableColumn id="3" xr3:uid="{21CA94C3-7296-4750-8C26-6BD6C36A79E4}" name="Interest Rate" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{21CA94C3-7296-4750-8C26-6BD6C36A79E4}" name="Interest Rate" dataDxfId="38" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{A9093FCB-6BEB-4E2E-9882-B237200196F3}" name="Months"/>
     <tableColumn id="5" xr3:uid="{B4853DA0-AA77-4178-81EC-38D22C579214}" name="Interest Paid">
       <calculatedColumnFormula>B4*C4</calculatedColumnFormula>
@@ -7151,7 +7217,7 @@
     <tableColumn id="6" xr3:uid="{FF4F7AB6-78F5-4286-A14B-7D915316EEE0}" name="Total Loan Amount">
       <calculatedColumnFormula>B4+E4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8FDD81AB-2AD0-4F99-B5EE-09CBA8B5F305}" name="Monthly Payment" dataDxfId="25">
+    <tableColumn id="7" xr3:uid="{8FDD81AB-2AD0-4F99-B5EE-09CBA8B5F305}" name="Monthly Payment" dataDxfId="37">
       <calculatedColumnFormula>F4/D4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7160,18 +7226,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7DA315A0-2974-435B-9981-7FB3778632D6}" name="Table4" displayName="Table4" ref="A2:I210" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13" headerRowBorderDxfId="23" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7DA315A0-2974-435B-9981-7FB3778632D6}" name="Table4" displayName="Table4" ref="A2:I210" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
   <autoFilter ref="A2:I210" xr:uid="{7DA315A0-2974-435B-9981-7FB3778632D6}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{1F885A81-3696-4EF8-9BD2-91BF4F7EFEF0}" name="Document Date" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{325EFA64-CA15-43CD-BAAE-07EF613BD1D9}" name="Supplier" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{DDD4B2C3-4F21-422C-AB36-C8A3D11525BE}" name="Reference" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{CB58A3DD-216E-421D-BBE5-A02D457939DD}" name="Description" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{C4047194-7D97-4F09-92AC-61647193B54F}" name="Tax Inclusive Amount" dataDxfId="18" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{2EA291C1-3E5C-422C-A58D-351173A7110B}" name="Column1" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{0B49AE2C-8529-44F1-B6B2-5B4BB2BA0D12}" name="Bank Code" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{D2D16770-5ABD-457F-A131-3CBC97D45A64}" name="Account Code" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{DA370255-740F-4536-81EB-B1387D89AF72}" name="Payment Date" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{1F885A81-3696-4EF8-9BD2-91BF4F7EFEF0}" name="Document Date" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{325EFA64-CA15-43CD-BAAE-07EF613BD1D9}" name="Supplier" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{DDD4B2C3-4F21-422C-AB36-C8A3D11525BE}" name="Reference" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{CB58A3DD-216E-421D-BBE5-A02D457939DD}" name="Description" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{C4047194-7D97-4F09-92AC-61647193B54F}" name="Tax Inclusive Amount" dataDxfId="28" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{2EA291C1-3E5C-422C-A58D-351173A7110B}" name="Column1" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{0B49AE2C-8529-44F1-B6B2-5B4BB2BA0D12}" name="Bank Code" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{D2D16770-5ABD-457F-A131-3CBC97D45A64}" name="Account Code" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{DA370255-740F-4536-81EB-B1387D89AF72}" name="Payment Date" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14044,13 +14110,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C43B33-F636-4756-A5CD-D89DC94C9218}">
-  <dimension ref="A3:E19"/>
+  <dimension ref="A3:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -14083,221 +14153,247 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
-        <v>40923</v>
+        <v>40910</v>
       </c>
       <c r="B5" s="26">
-        <v>80</v>
-      </c>
-      <c r="C5" s="26">
-        <v>35</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26">
-        <v>115</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
-        <v>40924</v>
+        <v>40913</v>
       </c>
       <c r="B6" s="26">
-        <v>1392</v>
+        <v>340</v>
       </c>
       <c r="C6" s="26"/>
-      <c r="D6" s="26">
-        <v>105</v>
-      </c>
+      <c r="D6" s="26"/>
       <c r="E6" s="26">
-        <v>1497</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
-        <v>40928</v>
+        <v>40923</v>
       </c>
       <c r="B7" s="26">
-        <v>20000</v>
+        <v>80</v>
       </c>
       <c r="C7" s="26">
-        <v>-20000</v>
+        <v>35</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
-        <v>40929</v>
-      </c>
-      <c r="B8" s="26"/>
+        <v>40924</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1392</v>
+      </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="E8" s="26">
-        <v>61</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
-        <v>40934</v>
+        <v>40928</v>
       </c>
       <c r="B9" s="26">
-        <v>6720</v>
+        <v>20000</v>
       </c>
       <c r="C9" s="26">
-        <v>20000</v>
+        <v>-20000</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26">
-        <v>26720</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
-        <v>40939</v>
-      </c>
-      <c r="B10" s="26">
-        <v>738.25</v>
-      </c>
+        <v>40929</v>
+      </c>
+      <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26">
-        <v>-170</v>
+        <v>61</v>
       </c>
       <c r="E10" s="26">
-        <v>568.25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
-        <v>40941</v>
+        <v>40934</v>
       </c>
       <c r="B11" s="26">
-        <v>1000</v>
-      </c>
-      <c r="C11" s="26"/>
+        <v>6720</v>
+      </c>
+      <c r="C11" s="26">
+        <v>20000</v>
+      </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26">
-        <v>1000</v>
+        <v>26720</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
-        <v>40944</v>
+        <v>40939</v>
       </c>
       <c r="B12" s="26">
-        <v>340</v>
+        <v>738.25</v>
       </c>
       <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="D12" s="26">
+        <v>-170</v>
+      </c>
       <c r="E12" s="26">
-        <v>340</v>
+        <v>568.25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
-        <v>40954</v>
+        <v>40941</v>
       </c>
       <c r="B13" s="26">
-        <v>80</v>
-      </c>
-      <c r="C13" s="26">
-        <v>35</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26">
-        <v>115</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
-        <v>40959</v>
+        <v>40944</v>
       </c>
       <c r="B14" s="26">
-        <v>20000</v>
-      </c>
-      <c r="C14" s="26">
-        <v>-20000</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="26">
-        <v>0</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
-        <v>40964</v>
+        <v>40954</v>
       </c>
       <c r="B15" s="26">
-        <v>2200</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26">
-        <v>75</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C15" s="26">
+        <v>35</v>
+      </c>
+      <c r="D15" s="26"/>
       <c r="E15" s="26">
-        <v>2275</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
-        <v>40965</v>
+        <v>40959</v>
       </c>
       <c r="B16" s="26">
-        <v>6720</v>
+        <v>20000</v>
       </c>
       <c r="C16" s="26">
-        <v>20000</v>
+        <v>-20000</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26">
-        <v>26720</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
-        <v>40966</v>
+        <v>40964</v>
       </c>
       <c r="B17" s="26">
-        <v>514</v>
+        <v>2200</v>
       </c>
       <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
+      <c r="D17" s="26">
+        <v>75</v>
+      </c>
       <c r="E17" s="26">
-        <v>514</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
+        <v>40965</v>
+      </c>
+      <c r="B18" s="26">
+        <v>6720</v>
+      </c>
+      <c r="C18" s="26">
+        <v>20000</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26">
+        <v>26720</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>40966</v>
+      </c>
+      <c r="B19" s="26">
+        <v>514</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
         <v>40968</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B20" s="26">
         <v>3770</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26">
         <v>-70</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E20" s="26">
         <v>3700</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="26">
-        <v>63554.25</v>
-      </c>
-      <c r="C19" s="26">
+      <c r="B21" s="26">
+        <v>64894.25</v>
+      </c>
+      <c r="C21" s="26">
         <v>70</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D21" s="26">
         <v>1</v>
       </c>
-      <c r="E19" s="26">
-        <v>63625.25</v>
+      <c r="E21" s="26">
+        <v>64965.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>